<commit_message>
back to use DRV8305 again, fxxk 8301's PWR_PAD
</commit_message>
<xml_diff>
--- a/motor_DRV8301/BOM_8301.xlsx
+++ b/motor_DRV8301/BOM_8301.xlsx
@@ -1016,7 +1016,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,6 +2294,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>